<commit_message>
added scenarios for yearly service row addition
</commit_message>
<xml_diff>
--- a/Utilities/YearlyServiceInputs.xlsx
+++ b/Utilities/YearlyServiceInputs.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SmartCliff-Admin-Project\Utilities\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9543D7D2-85BE-4201-99F8-A1A5CB39707A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="5760" yWindow="2424" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,82 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+  <si>
+    <t>${test_case_name}</t>
+  </si>
+  <si>
+    <t>add_valid</t>
+  </si>
+  <si>
+    <t>${year}</t>
+  </si>
+  <si>
+    <t>2021-2025</t>
+  </si>
+  <si>
+    <t>${bussiness}</t>
+  </si>
+  <si>
+    <t>${service1}</t>
+  </si>
+  <si>
+    <t>training</t>
+  </si>
+  <si>
+    <t>testing automation</t>
+  </si>
+  <si>
+    <t>${business2}</t>
+  </si>
+  <si>
+    <t>${service2}</t>
+  </si>
+  <si>
+    <t>delete_valid</t>
+  </si>
+  <si>
+    <t>2021-2026</t>
+  </si>
+  <si>
+    <t>csr</t>
+  </si>
+  <si>
+    <t>test servies for deletion</t>
+  </si>
+  <si>
+    <t>empty_year</t>
+  </si>
+  <si>
+    <t>sample test service</t>
+  </si>
+  <si>
+    <t>add_new_service</t>
+  </si>
+  <si>
+    <t>b2b</t>
+  </si>
+  <si>
+    <t>new service</t>
+  </si>
+  <si>
+    <t>del_new_service</t>
+  </si>
+  <si>
+    <t>crc</t>
+  </si>
+  <si>
+    <t>fullstack</t>
+  </si>
+  <si>
+    <t>deleted service</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +410,116 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>2024</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>